<commit_message>
Updated the way of fetching the data from the test data files
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataFiles/MV_TestData.xlsx
+++ b/src/test/resources/testDataFiles/MV_TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7325\git\MV_Selenium_Using_Shaft_Engine\src\test\java\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7325\Sample_Project_Using_Shaft_Engine\MV_WebApp_New_Syntax\src\test\resources\testDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D833235E-F51C-4667-9448-03E8F450D2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1703ADEB-71A7-4648-B7C4-ED587917F8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9375" yWindow="-14325" windowWidth="21600" windowHeight="11835" xr2:uid="{F9CDADB8-3C7A-4B96-B80B-F4BE14C35D5B}"/>
+    <workbookView xWindow="13935" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{F9CDADB8-3C7A-4B96-B80B-F4BE14C35D5B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MV_Testdaten_Iterations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>DE</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Kennzeichen</t>
+  </si>
+  <si>
+    <t>Buchungssprache</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Polski</t>
   </si>
 </sst>
 </file>
@@ -110,11 +119,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B2C706B3-B42B-47C4-B557-0E1262DAA214}" name="Zulassungsland"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B2C706B3-B42B-47C4-B557-0E1262DAA214}" name="Buchungssprache"/>
     <tableColumn id="2" xr3:uid="{3DB15357-4581-41C5-B49D-B9744F286021}" name="Kennzeichen"/>
+    <tableColumn id="3" xr3:uid="{F1654490-A9F8-4A62-B754-20A5C941841F}" name="Zulassungsland"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,46 +427,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ADEC2E-7C9B-4BFD-AACB-ECF2D50E95AB}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testbase and testng.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataFiles/MV_TestData.xlsx
+++ b/src/test/resources/testDataFiles/MV_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7325\Sample_Project_Using_Shaft_Engine\MV_WebApp_New_Syntax\src\test\resources\testDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1703ADEB-71A7-4648-B7C4-ED587917F8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFA8C63-1B18-4960-9FAE-818A8EE22831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13935" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{F9CDADB8-3C7A-4B96-B80B-F4BE14C35D5B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>DE</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Schadstoffklasse_Title_Soll</t>
+  </si>
+  <si>
+    <t>Schadstoffklasse</t>
+  </si>
+  <si>
+    <t>Klasa emisji spalin</t>
   </si>
   <si>
     <t>Polski</t>
@@ -119,12 +128,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{8E45C3FA-C640-4B8F-9083-C9F1B05DB5F9}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B2C706B3-B42B-47C4-B557-0E1262DAA214}" name="Buchungssprache"/>
-    <tableColumn id="2" xr3:uid="{3DB15357-4581-41C5-B49D-B9744F286021}" name="Kennzeichen"/>
-    <tableColumn id="3" xr3:uid="{F1654490-A9F8-4A62-B754-20A5C941841F}" name="Zulassungsland"/>
+    <tableColumn id="2" xr3:uid="{3DB15357-4581-41C5-B49D-B9744F286021}" name="Zulassungsland"/>
+    <tableColumn id="3" xr3:uid="{F1654490-A9F8-4A62-B754-20A5C941841F}" name="Kennzeichen"/>
+    <tableColumn id="4" xr3:uid="{FDC4E733-9BCC-4505-AB84-199182A52125}" name="Schadstoffklasse_Title_Soll"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -427,67 +437,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ADEC2E-7C9B-4BFD-AACB-ECF2D50E95AB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
+      <c r="D1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>